<commit_message>
Updated for beta build.
</commit_message>
<xml_diff>
--- a/eagle/bp/js220_bp_bom.xlsx
+++ b/eagle/bp/js220_bp_bom.xlsx
@@ -552,7 +552,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>2022 February 17</t>
+          <t>2022 June 16</t>
         </is>
       </c>
     </row>
@@ -574,7 +574,7 @@
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>Mfgr Part #</t>
+          <t>Name</t>
         </is>
       </c>
     </row>
@@ -592,7 +592,7 @@
       </c>
       <c r="D5" s="9" t="inlineStr">
         <is>
-          <t>JS220_fp_bp_pcb_revB</t>
+          <t>JS220_ep_pcb_revC</t>
         </is>
       </c>
     </row>
@@ -641,7 +641,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>2022 February 17</t>
+          <t>2022 June 16</t>
         </is>
       </c>
     </row>
@@ -663,7 +663,7 @@
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>Mfgr Part #</t>
+          <t>Name</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="D5" s="9" t="inlineStr">
         <is>
-          <t>JS220_fp_bp_pcb_revB</t>
+          <t>JS220_ep_pcb_revC</t>
         </is>
       </c>
     </row>
@@ -730,7 +730,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>2022 February 17</t>
+          <t>2022 June 16</t>
         </is>
       </c>
     </row>
@@ -752,7 +752,7 @@
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>Mfgr Part #</t>
+          <t>Name</t>
         </is>
       </c>
     </row>

</xml_diff>